<commit_message>
chicker works! (slight bug in code, but works)
- avoid kicking near when the next charge cycle starts (as it doesnt stop the pulse if a charge cycle starts after the pulse goes out). this will break the IGBT due to potential delays / and maybe current from charging idk
</commit_message>
<xml_diff>
--- a/Chicker/firmware/battery_offset.xlsx
+++ b/Chicker/firmware/battery_offset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The_Bots\Electrical\Chicker\firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B8B403-616E-438A-8AC7-19040BDABEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8144CB97-95A2-4E5B-9E6C-25823B0FA8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{7C04D6C3-C8BC-4281-B997-3C7E3B4806F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{7C04D6C3-C8BC-4281-B997-3C7E3B4806F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Actual Voltage</t>
   </si>
   <si>
     <t>Simulated Voltage</t>
+  </si>
+  <si>
+    <t>y = 1.0893x - 0.5781</t>
   </si>
 </sst>
 </file>
@@ -244,83 +247,65 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8810000000000002</c:v>
+                  <c:v>4.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3120000000000003</c:v>
+                  <c:v>6.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7430000000000003</c:v>
+                  <c:v>8.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1740000000000013</c:v>
+                  <c:v>10.64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.6050000000000022</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.036000000000003</c:v>
+                  <c:v>14.82</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.467000000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13.898000000000005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15.329000000000006</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16.760000000000002</c:v>
+                  <c:v>15.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.48</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.96</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4399999999999995</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.92</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.4</c:v>
+                  <c:v>13.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.88</c:v>
+                  <c:v>15.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.360000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13.840000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15.320000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>16.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -1554,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B105CA27-ACB7-48AC-9EE7-499FA0996779}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1566,7 +1551,7 @@
     <col min="3" max="3" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1574,154 +1559,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2.4500000000000002</v>
+        <v>3.1</v>
       </c>
       <c r="B2">
-        <f>A2/1.00614</f>
-        <v>2.4350488003657542</v>
+        <f t="shared" ref="B2:B9" si="0">A2/1.00614</f>
+        <v>3.081082155564832</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>2.8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>($A$12-$A$2)/10+A2</f>
-        <v>3.8810000000000002</v>
+        <v>4.45</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B12" si="0">A3/1.00614</f>
-        <v>3.8573160792732621</v>
+        <f t="shared" si="0"/>
+        <v>4.4228437394398394</v>
       </c>
       <c r="C3">
-        <f>($C$12-$C$2)/10+C2</f>
-        <v>3.48</v>
+        <v>4.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>($A$12-$A$2)/10+A3</f>
-        <v>5.3120000000000003</v>
+        <v>6.35</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>5.2795833581807701</v>
+        <v>6.31124893156022</v>
       </c>
       <c r="C4">
-        <f>($C$12-$C$2)/10+C3</f>
-        <v>4.96</v>
+        <v>6.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>($A$12-$A$2)/10+A4</f>
-        <v>6.7430000000000003</v>
+        <v>8.06</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>6.7018506370882784</v>
+        <v>8.0108136044685629</v>
       </c>
       <c r="C5">
-        <f>($C$12-$C$2)/10+C4</f>
-        <v>6.4399999999999995</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>($A$12-$A$2)/10+A5</f>
-        <v>8.1740000000000013</v>
+        <v>10.64</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>8.1241179159957877</v>
+        <v>10.575069075874133</v>
       </c>
       <c r="C6">
-        <f>($C$12-$C$2)/10+C5</f>
-        <v>7.92</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>($A$12-$A$2)/10+A6</f>
-        <v>9.6050000000000022</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>9.5463851949032961</v>
+        <v>12.920667103981552</v>
       </c>
       <c r="C7">
-        <f>($C$12-$C$2)/10+C6</f>
-        <v>9.4</v>
+        <v>13.6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>($A$12-$A$2)/10+A7</f>
-        <v>11.036000000000003</v>
+        <v>14.82</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>10.968652473810804</v>
+        <v>14.729560498538971</v>
       </c>
       <c r="C8">
-        <f>($C$12-$C$2)/10+C7</f>
-        <v>10.88</v>
+        <v>15.6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>($A$12-$A$2)/10+A8</f>
-        <v>12.467000000000004</v>
+        <v>15.98</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>12.390919752718313</v>
+        <v>15.88248156320194</v>
       </c>
       <c r="C9">
-        <f>($C$12-$C$2)/10+C8</f>
-        <v>12.360000000000001</v>
+        <v>16.8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f>($A$12-$A$2)/10+A9</f>
-        <v>13.898000000000005</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>13.813187031625821</v>
-      </c>
-      <c r="C10">
-        <f>($C$12-$C$2)/10+C9</f>
-        <v>13.840000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f>($A$12-$A$2)/10+A10</f>
-        <v>15.329000000000006</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>15.235454310533331</v>
-      </c>
-      <c r="C11">
-        <f>($C$12-$C$2)/10+C10</f>
-        <v>15.320000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>16.760000000000002</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>16.657721589440833</v>
-      </c>
-      <c r="C12">
-        <v>16.8</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>